<commit_message>
Updates to violin plots and combined config, as well as calculation of mu and sigma
</commit_message>
<xml_diff>
--- a/default_configs/updated_combined_config.xlsx
+++ b/default_configs/updated_combined_config.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q384"/>
+  <dimension ref="A1:R384"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,11 @@
       <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>comments</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 17</t>
         </is>
       </c>
     </row>
@@ -558,6 +563,7 @@
           <t>thermal value methane</t>
         </is>
       </c>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -593,6 +599,7 @@
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,6 +635,7 @@
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -667,6 +675,7 @@
           <t>at 0°C, 1 atm</t>
         </is>
       </c>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -706,6 +715,7 @@
           <t>at 0°C, 1 atm</t>
         </is>
       </c>
+      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -745,6 +755,7 @@
           <t>molar weight hydrogen</t>
         </is>
       </c>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -784,6 +795,7 @@
           <t>molar weight carbon</t>
         </is>
       </c>
+      <c r="R8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -823,6 +835,7 @@
           <t>molar weight oxygen</t>
         </is>
       </c>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -862,6 +875,7 @@
           <t>molar weight nitrogen</t>
         </is>
       </c>
+      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -901,6 +915,7 @@
           <t>molar weight methane</t>
         </is>
       </c>
+      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -940,6 +955,7 @@
           <t>molar weight co2</t>
         </is>
       </c>
+      <c r="R12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -979,6 +995,7 @@
           <t>molar weight n2o</t>
         </is>
       </c>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1018,6 +1035,7 @@
           <t>molar weight nh3</t>
         </is>
       </c>
+      <c r="R14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1049,6 +1067,7 @@
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1078,6 +1097,7 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1107,6 +1127,7 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1152,6 +1173,7 @@
           <t>GWP100 of methane in kg CO2 eq</t>
         </is>
       </c>
+      <c r="R18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1197,6 +1219,7 @@
           <t>GWP100 of N2O in kg CO2 eq</t>
         </is>
       </c>
+      <c r="R19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1242,6 +1265,7 @@
           <t>gwp 100 of diesel in kg CO2 eq</t>
         </is>
       </c>
+      <c r="R20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1287,6 +1311,7 @@
           <t>CO2 equivalent of the (swiss) electricity mix per kWh of electricity</t>
         </is>
       </c>
+      <c r="R21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1332,6 +1357,7 @@
           <t>CO2 equivalent of heating oil per kWh of heat</t>
         </is>
       </c>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1375,6 +1401,7 @@
           <t>GWP 100 of heating with natural gas per MJ of energy, according to Ecoinvent</t>
         </is>
       </c>
+      <c r="R23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1418,6 +1445,7 @@
           <t>GWP 100 of heating with oil per MJ of energy, according to Ecoinvent</t>
         </is>
       </c>
+      <c r="R24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1461,6 +1489,7 @@
           <t>GWP 100 of AD plant construction according to Ecoinvent (lifetime 20 years for construction, 10 years for machinery)</t>
         </is>
       </c>
+      <c r="R25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1504,6 +1533,7 @@
           <t>GWP 100 of CHP construction according to ecoinvent (Runtime 80'000 hours)</t>
         </is>
       </c>
+      <c r="R26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1549,6 +1579,7 @@
           <t>Swiss aggregated environmental impact factor (Umweltbelastungspunkte) for NH3 emissions into air</t>
         </is>
       </c>
+      <c r="R27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1594,6 +1625,7 @@
           <t>Swiss aggregated environmental impact factor (Umweltbelastungspunkte) for CO2 equivalent emissions into air</t>
         </is>
       </c>
+      <c r="R28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1639,6 +1671,7 @@
           <t>Swiss aggregated environmental impact factor (Umweltbelastungspunkte) for non renewable energy sources</t>
         </is>
       </c>
+      <c r="R29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1684,6 +1717,7 @@
           <t>Swiss aggregated environmental impact factor (Umweltbelastungspunkte) for renewable energy sources</t>
         </is>
       </c>
+      <c r="R30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1725,6 +1759,7 @@
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1766,6 +1801,7 @@
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1811,6 +1847,7 @@
           <t>Factor for operating time of CHP</t>
         </is>
       </c>
+      <c r="R33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1856,6 +1893,7 @@
           <t>fuel used is Diesel</t>
         </is>
       </c>
+      <c r="R34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1890,10 +1928,10 @@
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
-        <v>-0.8252970699546591</v>
+        <v>-0.7780521793311018</v>
       </c>
       <c r="O35" t="n">
-        <v>0.3574102646579123</v>
+        <v>0.1823521758458736</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
@@ -1905,6 +1943,7 @@
           <t>percentage of nitrogen from manure that is plant accessible</t>
         </is>
       </c>
+      <c r="R35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1939,10 +1978,10 @@
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="n">
-        <v>-0.720766229032606</v>
+        <v>-0.681350423821061</v>
       </c>
       <c r="O36" t="n">
-        <v>0.3264561079877</v>
+        <v>0.1665592387692347</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -1954,6 +1993,7 @@
           <t>percentage of nitrogen from digestate that is plant accessible</t>
         </is>
       </c>
+      <c r="R36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1988,10 +2028,10 @@
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="n">
-        <v>-0.9070395716385784</v>
+        <v>-0.8603875789742587</v>
       </c>
       <c r="O37" t="n">
-        <v>0.3551605308703359</v>
+        <v>0.1812043524848652</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
@@ -2003,6 +2043,7 @@
           <t>percentage of accessible Nitrogen that is released as NH3</t>
         </is>
       </c>
+      <c r="R37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2044,6 +2085,7 @@
           <t>reduction factor in NH3 emissions when using specific field application Method (here Schleppschlauch)</t>
         </is>
       </c>
+      <c r="R38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2074,10 +2116,10 @@
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="n">
-        <v>-0.6960169480781981</v>
+        <v>-0.5714645324811189</v>
       </c>
       <c r="O39" t="n">
-        <v>0.5803175096373125</v>
+        <v>0.2960803620598533</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
@@ -2085,6 +2127,7 @@
         </is>
       </c>
       <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2115,10 +2158,10 @@
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="n">
-        <v>-1.249719909038362</v>
+        <v>-1.081019391405987</v>
       </c>
       <c r="O40" t="n">
-        <v>0.6753793919070684</v>
+        <v>0.3445813224015655</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
@@ -2126,6 +2169,7 @@
         </is>
       </c>
       <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2161,6 +2205,7 @@
         </is>
       </c>
       <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2202,6 +2247,7 @@
           <t>nitrogen emitted as N2O, in percentage of (N accessible - N NH3)</t>
         </is>
       </c>
+      <c r="R42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2236,10 +2282,10 @@
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="n">
-        <v>-0.5807775972579186</v>
+        <v>-0.5290346964159095</v>
       </c>
       <c r="O43" t="n">
-        <v>0.3740373604118386</v>
+        <v>0.1908353879652238</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
@@ -2251,6 +2297,7 @@
           <t>methane content of Biogas from AD</t>
         </is>
       </c>
+      <c r="R43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2284,6 +2331,7 @@
           <t>CO2 content of Biogas from AD</t>
         </is>
       </c>
+      <c r="R44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2318,10 +2366,10 @@
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
-        <v>-7.57614372032182</v>
+        <v>-7.08174227433295</v>
       </c>
       <c r="O45" t="n">
-        <v>1.156190677474683</v>
+        <v>0.5898932027932058</v>
       </c>
       <c r="P45" t="inlineStr">
         <is>
@@ -2333,6 +2381,7 @@
           <t>percentage of total CH4 produced, that is lost during AD process</t>
         </is>
       </c>
+      <c r="R45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2384,6 +2433,7 @@
           <t>heat demand of an AD plant in relation to biogas produced</t>
         </is>
       </c>
+      <c r="R46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2435,6 +2485,7 @@
           <t>electricity demand of an AD plant in relation to biogas produced</t>
         </is>
       </c>
+      <c r="R47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2452,8 +2503,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
+      <c r="F48" t="n">
+        <v>3.8e-05</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2.6e-05</v>
+      </c>
       <c r="H48" t="n">
         <v>3.2e-05</v>
       </c>
@@ -2462,8 +2517,12 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
+      <c r="N48" t="n">
+        <v>-10.36212268794077</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.1571498188113268</v>
+      </c>
       <c r="P48" t="inlineStr">
         <is>
           <t>Amon et al.</t>
@@ -2472,6 +2531,11 @@
       <c r="Q48" t="inlineStr">
         <is>
           <t>daily percentage emissions of NH3 during storage of digestate (results in nh3-N)</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -2491,8 +2555,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
+      <c r="F49" t="n">
+        <v>4.3e-05</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2.9e-06</v>
+      </c>
       <c r="H49" t="n">
         <v>3.6e-06</v>
       </c>
@@ -2501,8 +2569,12 @@
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
+      <c r="N49" t="n">
+        <v>-12.62231650121984</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.4189028257666175</v>
+      </c>
       <c r="P49" t="inlineStr">
         <is>
           <t>Amon et al.</t>
@@ -2511,6 +2583,11 @@
       <c r="Q49" t="inlineStr">
         <is>
           <t>daily percentage emissions of N2O during storage of digestate (results in N2O-N)</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -2530,8 +2607,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>0.00072</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.00048</v>
+      </c>
       <c r="H50" t="n">
         <v>0.0005999999999999999</v>
       </c>
@@ -2540,8 +2621,12 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
+      <c r="N50" t="n">
+        <v>-7.431774139554022</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.1624391381773095</v>
+      </c>
       <c r="P50" t="inlineStr">
         <is>
           <t>Amon et al.</t>
@@ -2550,6 +2635,11 @@
       <c r="Q50" t="inlineStr">
         <is>
           <t>daily percentage emissions of CH4 during storage of digestate (results in CH4-C)</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -2569,8 +2659,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>0.00018</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.00012</v>
+      </c>
       <c r="H51" t="n">
         <v>0.00015</v>
       </c>
@@ -2579,8 +2673,12 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
+      <c r="N51" t="n">
+        <v>-8.818068500673911</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0.1624391381773095</v>
+      </c>
       <c r="P51" t="inlineStr">
         <is>
           <t>Amon et al.</t>
@@ -2589,6 +2687,11 @@
       <c r="Q51" t="inlineStr">
         <is>
           <t>daily percentage emissions of NH3 during storage of manure (results in NH3-N)</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -2610,8 +2713,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
+      <c r="F52" t="n">
+        <v>6.719999999999999e-05</v>
+      </c>
+      <c r="G52" t="n">
+        <v>4.48e-05</v>
+      </c>
       <c r="H52" t="n">
         <v>5.6e-05</v>
       </c>
@@ -2620,8 +2727,12 @@
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
+      <c r="N52" t="n">
+        <v>-9.803352104035019</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0.1624391381773095</v>
+      </c>
       <c r="P52" t="inlineStr">
         <is>
           <t>Amon et al.</t>
@@ -2630,6 +2741,11 @@
       <c r="Q52" t="inlineStr">
         <is>
           <t>daily percentage emissions of N2O during storage of manure (results in N2O-N)</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -2651,8 +2767,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>0.00132</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.00088</v>
+      </c>
       <c r="H53" t="n">
         <v>0.0011</v>
       </c>
@@ -2661,8 +2781,12 @@
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
+      <c r="N53" t="n">
+        <v>-6.825638335983705</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.1624391381773095</v>
+      </c>
       <c r="P53" t="inlineStr">
         <is>
           <t>Amon et al.</t>
@@ -2671,6 +2795,11 @@
       <c r="Q53" t="inlineStr">
         <is>
           <t>daily percentage emissions of CH4 during storage of manure (results in CH4-C)</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -2716,6 +2845,7 @@
           <t>factor, by which the methane potential increases after steam pretreatment</t>
         </is>
       </c>
+      <c r="R54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2752,10 +2882,10 @@
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="n">
-        <v>-0.830473716643459</v>
+        <v>-0.7288944046549873</v>
       </c>
       <c r="O55" t="n">
-        <v>0.5240735369841024</v>
+        <v>0.2673844576449502</v>
       </c>
       <c r="P55" t="inlineStr">
         <is>
@@ -2767,6 +2897,7 @@
           <t>Energy (heat) demand of steam treatment per kg of manure/straw</t>
         </is>
       </c>
+      <c r="R55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2806,6 +2937,7 @@
           <t>percentage of total biogas that is used in biogas upgrading</t>
         </is>
       </c>
+      <c r="R56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2845,6 +2977,7 @@
           <t>percentage of total biogas that is used for energy production in a CHP</t>
         </is>
       </c>
+      <c r="R57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2866,8 +2999,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>0.348</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.232</v>
+      </c>
       <c r="H58" t="n">
         <v>0.29</v>
       </c>
@@ -2876,8 +3013,12 @@
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
       <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr"/>
+      <c r="N58" t="n">
+        <v>-1.251067592807511</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.1624391381773095</v>
+      </c>
       <c r="P58" t="inlineStr">
         <is>
           <t>Ardolino et al.</t>
@@ -2886,6 +3027,11 @@
       <c r="Q58" t="inlineStr">
         <is>
           <t>electricity cost for biogas upgrading per m3 of biogas going in</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -2902,11 +3048,15 @@
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>lognormal</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+          <t>Triangle</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.95</v>
+      </c>
       <c r="H59" t="n">
         <v>0.9747</v>
       </c>
@@ -2927,6 +3077,11 @@
           <t>methane content of the upgraded product (biomethane)</t>
         </is>
       </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2941,7 +3096,7 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>lognormal</t>
+          <t>none</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -2966,6 +3121,11 @@
           <t>co2 content of biomethane after the upgrading process</t>
         </is>
       </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2983,8 +3143,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+      <c r="F61" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.36</v>
+      </c>
       <c r="H61" t="n">
         <v>0.4</v>
       </c>
@@ -2993,8 +3157,12 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
-      <c r="O61" t="inlineStr"/>
+      <c r="N61" t="n">
+        <v>-0.9228202604384951</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0.1142762316874344</v>
+      </c>
       <c r="P61" t="inlineStr">
         <is>
           <t>Ardolino et al.</t>
@@ -3003,6 +3171,11 @@
       <c r="Q61" t="inlineStr">
         <is>
           <t>methane content of mixture of Biogas and Flugas going to the CHP generator</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 10% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -3022,8 +3195,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
+      <c r="F62" t="n">
+        <v>0.0083</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.0055</v>
+      </c>
       <c r="H62" t="n">
         <v>0.0069</v>
       </c>
@@ -3032,8 +3209,12 @@
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
       <c r="M62" t="inlineStr"/>
-      <c r="N62" t="inlineStr"/>
-      <c r="O62" t="inlineStr"/>
+      <c r="N62" t="n">
+        <v>-4.989623712188512</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0.1636450109816287</v>
+      </c>
       <c r="P62" t="inlineStr">
         <is>
           <t>Ardolino et al.</t>
@@ -3042,6 +3223,11 @@
       <c r="Q62" t="inlineStr">
         <is>
           <t>percentage of methane lost during upgrading process</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -3061,8 +3247,12 @@
           <t>lognormal</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>0.009480000000000001</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.0063</v>
+      </c>
       <c r="H63" t="n">
         <v>0.007900000000000001</v>
       </c>
@@ -3071,8 +3261,12 @@
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
       <c r="M63" t="inlineStr"/>
-      <c r="N63" t="inlineStr"/>
-      <c r="O63" t="inlineStr"/>
+      <c r="N63" t="n">
+        <v>-4.854188889604611</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0.1630728064114304</v>
+      </c>
       <c r="P63" t="inlineStr">
         <is>
           <t>Ardolino et al.</t>
@@ -3081,6 +3275,11 @@
       <c r="Q63" t="inlineStr">
         <is>
           <t>methane content of offgas after the upgrading process</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3296,7 @@
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>lognormal</t>
+          <t>none</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -3122,6 +3321,11 @@
           <t>co2 content of offgas after the upgrading process</t>
         </is>
       </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>Uncertainty factor is assumption by author (+- 20% for upper and lower limit)</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3136,7 +3340,7 @@
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>lognormal</t>
+          <t>none</t>
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
@@ -3157,6 +3361,7 @@
           <t>ratio of methane to co2 in the biomethane, for further calculations</t>
         </is>
       </c>
+      <c r="R65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3202,6 +3407,7 @@
           <t>efficiency of an AD plant depending on its size</t>
         </is>
       </c>
+      <c r="R66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3247,6 +3453,7 @@
           <t>efficiency of an AD plant depending on its size</t>
         </is>
       </c>
+      <c r="R67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3292,6 +3499,7 @@
           <t>efficiency of an AD plant depending on its size</t>
         </is>
       </c>
+      <c r="R68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3326,10 +3534,10 @@
       <c r="L69" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="n">
-        <v>-0.407358082452253</v>
+        <v>-0.369868180744626</v>
       </c>
       <c r="O69" t="n">
-        <v>0.3183807108275265</v>
+        <v>0.1624391381773095</v>
       </c>
       <c r="P69" t="inlineStr">
         <is>
@@ -3341,6 +3549,7 @@
           <t>efficiency of converting energy potential into electricity for a solid oxide fuel cell using methane</t>
         </is>
       </c>
+      <c r="R69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr"/>
@@ -3360,6 +3569,7 @@
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
       <c r="Q70" t="inlineStr"/>
+      <c r="R70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr"/>
@@ -3383,6 +3593,7 @@
           <t>Explanation for naming of animal config factors: [Animal type] + [Stable type] + [variable name]</t>
         </is>
       </c>
+      <c r="R71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr"/>
@@ -3406,6 +3617,7 @@
           <t>Stable types: 0 = only liquid manure collected, 1 = Solid, liquid and bedding collected, 2 = only solid and bedding collected</t>
         </is>
       </c>
+      <c r="R72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3441,6 +3653,7 @@
         </is>
       </c>
       <c r="Q73" t="inlineStr"/>
+      <c r="R73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3480,6 +3693,7 @@
         </is>
       </c>
       <c r="Q74" t="inlineStr"/>
+      <c r="R74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3519,6 +3733,7 @@
         </is>
       </c>
       <c r="Q75" t="inlineStr"/>
+      <c r="R75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3564,6 +3779,7 @@
         </is>
       </c>
       <c r="Q76" t="inlineStr"/>
+      <c r="R76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3609,6 +3825,7 @@
         </is>
       </c>
       <c r="Q77" t="inlineStr"/>
+      <c r="R77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3641,10 +3858,10 @@
       <c r="L78" t="inlineStr"/>
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O78" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P78" t="inlineStr">
         <is>
@@ -3652,6 +3869,7 @@
         </is>
       </c>
       <c r="Q78" t="inlineStr"/>
+      <c r="R78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3695,6 +3913,7 @@
         </is>
       </c>
       <c r="Q79" t="inlineStr"/>
+      <c r="R79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3740,6 +3959,7 @@
         </is>
       </c>
       <c r="Q80" t="inlineStr"/>
+      <c r="R80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3785,6 +4005,7 @@
         </is>
       </c>
       <c r="Q81" t="inlineStr"/>
+      <c r="R81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3830,6 +4051,7 @@
         </is>
       </c>
       <c r="Q82" t="inlineStr"/>
+      <c r="R82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3875,6 +4097,7 @@
         </is>
       </c>
       <c r="Q83" t="inlineStr"/>
+      <c r="R83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3910,6 +4133,7 @@
         </is>
       </c>
       <c r="Q84" t="inlineStr"/>
+      <c r="R84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3945,6 +4169,7 @@
         </is>
       </c>
       <c r="Q85" t="inlineStr"/>
+      <c r="R85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3980,6 +4205,7 @@
         </is>
       </c>
       <c r="Q86" t="inlineStr"/>
+      <c r="R86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4015,6 +4241,7 @@
         </is>
       </c>
       <c r="Q87" t="inlineStr"/>
+      <c r="R87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4060,6 +4287,7 @@
         </is>
       </c>
       <c r="Q88" t="inlineStr"/>
+      <c r="R88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4105,6 +4333,7 @@
         </is>
       </c>
       <c r="Q89" t="inlineStr"/>
+      <c r="R89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4137,10 +4366,10 @@
       <c r="L90" t="inlineStr"/>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O90" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P90" t="inlineStr">
         <is>
@@ -4148,6 +4377,7 @@
         </is>
       </c>
       <c r="Q90" t="inlineStr"/>
+      <c r="R90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4191,6 +4421,7 @@
         </is>
       </c>
       <c r="Q91" t="inlineStr"/>
+      <c r="R91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4236,6 +4467,7 @@
         </is>
       </c>
       <c r="Q92" t="inlineStr"/>
+      <c r="R92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4281,6 +4513,7 @@
         </is>
       </c>
       <c r="Q93" t="inlineStr"/>
+      <c r="R93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4326,6 +4559,7 @@
         </is>
       </c>
       <c r="Q94" t="inlineStr"/>
+      <c r="R94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4371,6 +4605,7 @@
         </is>
       </c>
       <c r="Q95" t="inlineStr"/>
+      <c r="R95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4406,6 +4641,7 @@
         </is>
       </c>
       <c r="Q96" t="inlineStr"/>
+      <c r="R96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4445,6 +4681,7 @@
         </is>
       </c>
       <c r="Q97" t="inlineStr"/>
+      <c r="R97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4480,6 +4717,7 @@
         </is>
       </c>
       <c r="Q98" t="inlineStr"/>
+      <c r="R98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4515,6 +4753,7 @@
         </is>
       </c>
       <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4560,6 +4799,7 @@
         </is>
       </c>
       <c r="Q100" t="inlineStr"/>
+      <c r="R100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4605,6 +4845,7 @@
         </is>
       </c>
       <c r="Q101" t="inlineStr"/>
+      <c r="R101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4637,10 +4878,10 @@
       <c r="L102" t="inlineStr"/>
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O102" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P102" t="inlineStr">
         <is>
@@ -4648,6 +4889,7 @@
         </is>
       </c>
       <c r="Q102" t="inlineStr"/>
+      <c r="R102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4691,6 +4933,7 @@
         </is>
       </c>
       <c r="Q103" t="inlineStr"/>
+      <c r="R103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4736,6 +4979,7 @@
         </is>
       </c>
       <c r="Q104" t="inlineStr"/>
+      <c r="R104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4781,6 +5025,7 @@
         </is>
       </c>
       <c r="Q105" t="inlineStr"/>
+      <c r="R105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4826,6 +5071,7 @@
         </is>
       </c>
       <c r="Q106" t="inlineStr"/>
+      <c r="R106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4871,6 +5117,7 @@
         </is>
       </c>
       <c r="Q107" t="inlineStr"/>
+      <c r="R107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4906,6 +5153,7 @@
         </is>
       </c>
       <c r="Q108" t="inlineStr"/>
+      <c r="R108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4941,6 +5189,7 @@
         </is>
       </c>
       <c r="Q109" t="inlineStr"/>
+      <c r="R109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4976,6 +5225,7 @@
         </is>
       </c>
       <c r="Q110" t="inlineStr"/>
+      <c r="R110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5011,6 +5261,7 @@
         </is>
       </c>
       <c r="Q111" t="inlineStr"/>
+      <c r="R111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5056,6 +5307,7 @@
         </is>
       </c>
       <c r="Q112" t="inlineStr"/>
+      <c r="R112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5101,6 +5353,7 @@
         </is>
       </c>
       <c r="Q113" t="inlineStr"/>
+      <c r="R113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5133,10 +5386,10 @@
       <c r="L114" t="inlineStr"/>
       <c r="M114" t="inlineStr"/>
       <c r="N114" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O114" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P114" t="inlineStr">
         <is>
@@ -5144,6 +5397,7 @@
         </is>
       </c>
       <c r="Q114" t="inlineStr"/>
+      <c r="R114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5187,6 +5441,7 @@
         </is>
       </c>
       <c r="Q115" t="inlineStr"/>
+      <c r="R115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5232,6 +5487,7 @@
         </is>
       </c>
       <c r="Q116" t="inlineStr"/>
+      <c r="R116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5277,6 +5533,7 @@
         </is>
       </c>
       <c r="Q117" t="inlineStr"/>
+      <c r="R117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5322,6 +5579,7 @@
         </is>
       </c>
       <c r="Q118" t="inlineStr"/>
+      <c r="R118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5367,6 +5625,7 @@
         </is>
       </c>
       <c r="Q119" t="inlineStr"/>
+      <c r="R119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5402,6 +5661,7 @@
         </is>
       </c>
       <c r="Q120" t="inlineStr"/>
+      <c r="R120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5437,6 +5697,7 @@
         </is>
       </c>
       <c r="Q121" t="inlineStr"/>
+      <c r="R121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5472,6 +5733,7 @@
         </is>
       </c>
       <c r="Q122" t="inlineStr"/>
+      <c r="R122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5507,6 +5769,7 @@
         </is>
       </c>
       <c r="Q123" t="inlineStr"/>
+      <c r="R123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5552,6 +5815,7 @@
         </is>
       </c>
       <c r="Q124" t="inlineStr"/>
+      <c r="R124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5597,6 +5861,7 @@
         </is>
       </c>
       <c r="Q125" t="inlineStr"/>
+      <c r="R125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5629,10 +5894,10 @@
       <c r="L126" t="inlineStr"/>
       <c r="M126" t="inlineStr"/>
       <c r="N126" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O126" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P126" t="inlineStr">
         <is>
@@ -5640,6 +5905,7 @@
         </is>
       </c>
       <c r="Q126" t="inlineStr"/>
+      <c r="R126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5683,6 +5949,7 @@
         </is>
       </c>
       <c r="Q127" t="inlineStr"/>
+      <c r="R127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5728,6 +5995,7 @@
         </is>
       </c>
       <c r="Q128" t="inlineStr"/>
+      <c r="R128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5773,6 +6041,7 @@
         </is>
       </c>
       <c r="Q129" t="inlineStr"/>
+      <c r="R129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5818,6 +6087,7 @@
         </is>
       </c>
       <c r="Q130" t="inlineStr"/>
+      <c r="R130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5863,6 +6133,7 @@
         </is>
       </c>
       <c r="Q131" t="inlineStr"/>
+      <c r="R131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5898,6 +6169,7 @@
         </is>
       </c>
       <c r="Q132" t="inlineStr"/>
+      <c r="R132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5933,6 +6205,7 @@
         </is>
       </c>
       <c r="Q133" t="inlineStr"/>
+      <c r="R133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5968,6 +6241,7 @@
         </is>
       </c>
       <c r="Q134" t="inlineStr"/>
+      <c r="R134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -6003,6 +6277,7 @@
         </is>
       </c>
       <c r="Q135" t="inlineStr"/>
+      <c r="R135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6048,6 +6323,7 @@
         </is>
       </c>
       <c r="Q136" t="inlineStr"/>
+      <c r="R136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -6093,6 +6369,7 @@
         </is>
       </c>
       <c r="Q137" t="inlineStr"/>
+      <c r="R137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -6125,10 +6402,10 @@
       <c r="L138" t="inlineStr"/>
       <c r="M138" t="inlineStr"/>
       <c r="N138" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O138" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P138" t="inlineStr">
         <is>
@@ -6136,6 +6413,7 @@
         </is>
       </c>
       <c r="Q138" t="inlineStr"/>
+      <c r="R138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -6179,6 +6457,7 @@
         </is>
       </c>
       <c r="Q139" t="inlineStr"/>
+      <c r="R139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -6224,6 +6503,7 @@
         </is>
       </c>
       <c r="Q140" t="inlineStr"/>
+      <c r="R140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -6269,6 +6549,7 @@
         </is>
       </c>
       <c r="Q141" t="inlineStr"/>
+      <c r="R141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -6314,6 +6595,7 @@
         </is>
       </c>
       <c r="Q142" t="inlineStr"/>
+      <c r="R142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -6359,6 +6641,7 @@
         </is>
       </c>
       <c r="Q143" t="inlineStr"/>
+      <c r="R143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -6394,6 +6677,7 @@
         </is>
       </c>
       <c r="Q144" t="inlineStr"/>
+      <c r="R144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6429,6 +6713,7 @@
         </is>
       </c>
       <c r="Q145" t="inlineStr"/>
+      <c r="R145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -6464,6 +6749,7 @@
         </is>
       </c>
       <c r="Q146" t="inlineStr"/>
+      <c r="R146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6499,6 +6785,7 @@
         </is>
       </c>
       <c r="Q147" t="inlineStr"/>
+      <c r="R147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6544,6 +6831,7 @@
         </is>
       </c>
       <c r="Q148" t="inlineStr"/>
+      <c r="R148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -6589,6 +6877,7 @@
         </is>
       </c>
       <c r="Q149" t="inlineStr"/>
+      <c r="R149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6621,10 +6910,10 @@
       <c r="L150" t="inlineStr"/>
       <c r="M150" t="inlineStr"/>
       <c r="N150" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O150" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P150" t="inlineStr">
         <is>
@@ -6632,6 +6921,7 @@
         </is>
       </c>
       <c r="Q150" t="inlineStr"/>
+      <c r="R150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6675,6 +6965,7 @@
         </is>
       </c>
       <c r="Q151" t="inlineStr"/>
+      <c r="R151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6720,6 +7011,7 @@
         </is>
       </c>
       <c r="Q152" t="inlineStr"/>
+      <c r="R152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6765,6 +7057,7 @@
         </is>
       </c>
       <c r="Q153" t="inlineStr"/>
+      <c r="R153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6810,6 +7103,7 @@
         </is>
       </c>
       <c r="Q154" t="inlineStr"/>
+      <c r="R154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6855,6 +7149,7 @@
         </is>
       </c>
       <c r="Q155" t="inlineStr"/>
+      <c r="R155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6890,6 +7185,7 @@
         </is>
       </c>
       <c r="Q156" t="inlineStr"/>
+      <c r="R156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -6925,6 +7221,7 @@
         </is>
       </c>
       <c r="Q157" t="inlineStr"/>
+      <c r="R157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6960,6 +7257,7 @@
         </is>
       </c>
       <c r="Q158" t="inlineStr"/>
+      <c r="R158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6995,6 +7293,7 @@
         </is>
       </c>
       <c r="Q159" t="inlineStr"/>
+      <c r="R159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -7040,6 +7339,7 @@
         </is>
       </c>
       <c r="Q160" t="inlineStr"/>
+      <c r="R160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -7085,6 +7385,7 @@
         </is>
       </c>
       <c r="Q161" t="inlineStr"/>
+      <c r="R161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -7117,10 +7418,10 @@
       <c r="L162" t="inlineStr"/>
       <c r="M162" t="inlineStr"/>
       <c r="N162" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O162" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P162" t="inlineStr">
         <is>
@@ -7128,6 +7429,7 @@
         </is>
       </c>
       <c r="Q162" t="inlineStr"/>
+      <c r="R162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -7171,6 +7473,7 @@
         </is>
       </c>
       <c r="Q163" t="inlineStr"/>
+      <c r="R163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -7216,6 +7519,7 @@
         </is>
       </c>
       <c r="Q164" t="inlineStr"/>
+      <c r="R164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -7261,6 +7565,7 @@
         </is>
       </c>
       <c r="Q165" t="inlineStr"/>
+      <c r="R165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -7306,6 +7611,7 @@
         </is>
       </c>
       <c r="Q166" t="inlineStr"/>
+      <c r="R166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -7351,6 +7657,7 @@
         </is>
       </c>
       <c r="Q167" t="inlineStr"/>
+      <c r="R167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -7386,6 +7693,7 @@
         </is>
       </c>
       <c r="Q168" t="inlineStr"/>
+      <c r="R168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -7421,6 +7729,7 @@
         </is>
       </c>
       <c r="Q169" t="inlineStr"/>
+      <c r="R169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -7456,6 +7765,7 @@
         </is>
       </c>
       <c r="Q170" t="inlineStr"/>
+      <c r="R170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -7491,6 +7801,7 @@
         </is>
       </c>
       <c r="Q171" t="inlineStr"/>
+      <c r="R171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -7536,6 +7847,7 @@
         </is>
       </c>
       <c r="Q172" t="inlineStr"/>
+      <c r="R172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -7581,6 +7893,7 @@
         </is>
       </c>
       <c r="Q173" t="inlineStr"/>
+      <c r="R173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7613,10 +7926,10 @@
       <c r="L174" t="inlineStr"/>
       <c r="M174" t="inlineStr"/>
       <c r="N174" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O174" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P174" t="inlineStr">
         <is>
@@ -7624,6 +7937,7 @@
         </is>
       </c>
       <c r="Q174" t="inlineStr"/>
+      <c r="R174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -7667,6 +7981,7 @@
         </is>
       </c>
       <c r="Q175" t="inlineStr"/>
+      <c r="R175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -7712,6 +8027,7 @@
         </is>
       </c>
       <c r="Q176" t="inlineStr"/>
+      <c r="R176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -7757,6 +8073,7 @@
         </is>
       </c>
       <c r="Q177" t="inlineStr"/>
+      <c r="R177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -7802,6 +8119,7 @@
         </is>
       </c>
       <c r="Q178" t="inlineStr"/>
+      <c r="R178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -7847,6 +8165,7 @@
         </is>
       </c>
       <c r="Q179" t="inlineStr"/>
+      <c r="R179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -7882,6 +8201,7 @@
         </is>
       </c>
       <c r="Q180" t="inlineStr"/>
+      <c r="R180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -7917,6 +8237,7 @@
         </is>
       </c>
       <c r="Q181" t="inlineStr"/>
+      <c r="R181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -7952,6 +8273,7 @@
         </is>
       </c>
       <c r="Q182" t="inlineStr"/>
+      <c r="R182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -7987,6 +8309,7 @@
         </is>
       </c>
       <c r="Q183" t="inlineStr"/>
+      <c r="R183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -8032,6 +8355,7 @@
         </is>
       </c>
       <c r="Q184" t="inlineStr"/>
+      <c r="R184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -8077,6 +8401,7 @@
         </is>
       </c>
       <c r="Q185" t="inlineStr"/>
+      <c r="R185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -8109,10 +8434,10 @@
       <c r="L186" t="inlineStr"/>
       <c r="M186" t="inlineStr"/>
       <c r="N186" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O186" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P186" t="inlineStr">
         <is>
@@ -8120,6 +8445,7 @@
         </is>
       </c>
       <c r="Q186" t="inlineStr"/>
+      <c r="R186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -8163,6 +8489,7 @@
         </is>
       </c>
       <c r="Q187" t="inlineStr"/>
+      <c r="R187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -8208,6 +8535,7 @@
         </is>
       </c>
       <c r="Q188" t="inlineStr"/>
+      <c r="R188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -8253,6 +8581,7 @@
         </is>
       </c>
       <c r="Q189" t="inlineStr"/>
+      <c r="R189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -8298,6 +8627,7 @@
         </is>
       </c>
       <c r="Q190" t="inlineStr"/>
+      <c r="R190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -8343,6 +8673,7 @@
         </is>
       </c>
       <c r="Q191" t="inlineStr"/>
+      <c r="R191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -8378,6 +8709,7 @@
         </is>
       </c>
       <c r="Q192" t="inlineStr"/>
+      <c r="R192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -8413,6 +8745,7 @@
         </is>
       </c>
       <c r="Q193" t="inlineStr"/>
+      <c r="R193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -8448,6 +8781,7 @@
         </is>
       </c>
       <c r="Q194" t="inlineStr"/>
+      <c r="R194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -8483,6 +8817,7 @@
         </is>
       </c>
       <c r="Q195" t="inlineStr"/>
+      <c r="R195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -8528,6 +8863,7 @@
         </is>
       </c>
       <c r="Q196" t="inlineStr"/>
+      <c r="R196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -8573,6 +8909,7 @@
         </is>
       </c>
       <c r="Q197" t="inlineStr"/>
+      <c r="R197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -8605,10 +8942,10 @@
       <c r="L198" t="inlineStr"/>
       <c r="M198" t="inlineStr"/>
       <c r="N198" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O198" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P198" t="inlineStr">
         <is>
@@ -8616,6 +8953,7 @@
         </is>
       </c>
       <c r="Q198" t="inlineStr"/>
+      <c r="R198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -8659,6 +8997,7 @@
         </is>
       </c>
       <c r="Q199" t="inlineStr"/>
+      <c r="R199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -8704,6 +9043,7 @@
         </is>
       </c>
       <c r="Q200" t="inlineStr"/>
+      <c r="R200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -8749,6 +9089,7 @@
         </is>
       </c>
       <c r="Q201" t="inlineStr"/>
+      <c r="R201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -8794,6 +9135,7 @@
         </is>
       </c>
       <c r="Q202" t="inlineStr"/>
+      <c r="R202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -8839,6 +9181,7 @@
         </is>
       </c>
       <c r="Q203" t="inlineStr"/>
+      <c r="R203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -8874,6 +9217,7 @@
         </is>
       </c>
       <c r="Q204" t="inlineStr"/>
+      <c r="R204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -8909,6 +9253,7 @@
         </is>
       </c>
       <c r="Q205" t="inlineStr"/>
+      <c r="R205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -8944,6 +9289,7 @@
         </is>
       </c>
       <c r="Q206" t="inlineStr"/>
+      <c r="R206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -8979,6 +9325,7 @@
         </is>
       </c>
       <c r="Q207" t="inlineStr"/>
+      <c r="R207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -9024,6 +9371,7 @@
         </is>
       </c>
       <c r="Q208" t="inlineStr"/>
+      <c r="R208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -9069,6 +9417,7 @@
         </is>
       </c>
       <c r="Q209" t="inlineStr"/>
+      <c r="R209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -9101,10 +9450,10 @@
       <c r="L210" t="inlineStr"/>
       <c r="M210" t="inlineStr"/>
       <c r="N210" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O210" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P210" t="inlineStr">
         <is>
@@ -9112,6 +9461,7 @@
         </is>
       </c>
       <c r="Q210" t="inlineStr"/>
+      <c r="R210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -9155,6 +9505,7 @@
         </is>
       </c>
       <c r="Q211" t="inlineStr"/>
+      <c r="R211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -9200,6 +9551,7 @@
         </is>
       </c>
       <c r="Q212" t="inlineStr"/>
+      <c r="R212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -9245,6 +9597,7 @@
         </is>
       </c>
       <c r="Q213" t="inlineStr"/>
+      <c r="R213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -9290,6 +9643,7 @@
         </is>
       </c>
       <c r="Q214" t="inlineStr"/>
+      <c r="R214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -9335,6 +9689,7 @@
         </is>
       </c>
       <c r="Q215" t="inlineStr"/>
+      <c r="R215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -9370,6 +9725,7 @@
         </is>
       </c>
       <c r="Q216" t="inlineStr"/>
+      <c r="R216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -9405,6 +9761,7 @@
         </is>
       </c>
       <c r="Q217" t="inlineStr"/>
+      <c r="R217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -9440,6 +9797,7 @@
         </is>
       </c>
       <c r="Q218" t="inlineStr"/>
+      <c r="R218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -9475,6 +9833,7 @@
         </is>
       </c>
       <c r="Q219" t="inlineStr"/>
+      <c r="R219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -9520,6 +9879,7 @@
         </is>
       </c>
       <c r="Q220" t="inlineStr"/>
+      <c r="R220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -9565,6 +9925,7 @@
         </is>
       </c>
       <c r="Q221" t="inlineStr"/>
+      <c r="R221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -9597,10 +9958,10 @@
       <c r="L222" t="inlineStr"/>
       <c r="M222" t="inlineStr"/>
       <c r="N222" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O222" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P222" t="inlineStr">
         <is>
@@ -9608,6 +9969,7 @@
         </is>
       </c>
       <c r="Q222" t="inlineStr"/>
+      <c r="R222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -9651,6 +10013,7 @@
         </is>
       </c>
       <c r="Q223" t="inlineStr"/>
+      <c r="R223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -9696,6 +10059,7 @@
         </is>
       </c>
       <c r="Q224" t="inlineStr"/>
+      <c r="R224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -9741,6 +10105,7 @@
         </is>
       </c>
       <c r="Q225" t="inlineStr"/>
+      <c r="R225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -9786,6 +10151,7 @@
         </is>
       </c>
       <c r="Q226" t="inlineStr"/>
+      <c r="R226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -9831,6 +10197,7 @@
         </is>
       </c>
       <c r="Q227" t="inlineStr"/>
+      <c r="R227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -9866,6 +10233,7 @@
         </is>
       </c>
       <c r="Q228" t="inlineStr"/>
+      <c r="R228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -9901,6 +10269,7 @@
         </is>
       </c>
       <c r="Q229" t="inlineStr"/>
+      <c r="R229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -9936,6 +10305,7 @@
         </is>
       </c>
       <c r="Q230" t="inlineStr"/>
+      <c r="R230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -9971,6 +10341,7 @@
         </is>
       </c>
       <c r="Q231" t="inlineStr"/>
+      <c r="R231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -10016,6 +10387,7 @@
         </is>
       </c>
       <c r="Q232" t="inlineStr"/>
+      <c r="R232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -10061,6 +10433,7 @@
         </is>
       </c>
       <c r="Q233" t="inlineStr"/>
+      <c r="R233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -10093,10 +10466,10 @@
       <c r="L234" t="inlineStr"/>
       <c r="M234" t="inlineStr"/>
       <c r="N234" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O234" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P234" t="inlineStr">
         <is>
@@ -10104,6 +10477,7 @@
         </is>
       </c>
       <c r="Q234" t="inlineStr"/>
+      <c r="R234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -10147,6 +10521,7 @@
         </is>
       </c>
       <c r="Q235" t="inlineStr"/>
+      <c r="R235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -10192,6 +10567,7 @@
         </is>
       </c>
       <c r="Q236" t="inlineStr"/>
+      <c r="R236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -10237,6 +10613,7 @@
         </is>
       </c>
       <c r="Q237" t="inlineStr"/>
+      <c r="R237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -10282,6 +10659,7 @@
         </is>
       </c>
       <c r="Q238" t="inlineStr"/>
+      <c r="R238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -10327,6 +10705,7 @@
         </is>
       </c>
       <c r="Q239" t="inlineStr"/>
+      <c r="R239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -10362,6 +10741,7 @@
         </is>
       </c>
       <c r="Q240" t="inlineStr"/>
+      <c r="R240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -10397,6 +10777,7 @@
         </is>
       </c>
       <c r="Q241" t="inlineStr"/>
+      <c r="R241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -10432,6 +10813,7 @@
         </is>
       </c>
       <c r="Q242" t="inlineStr"/>
+      <c r="R242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -10467,6 +10849,7 @@
         </is>
       </c>
       <c r="Q243" t="inlineStr"/>
+      <c r="R243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -10512,6 +10895,7 @@
         </is>
       </c>
       <c r="Q244" t="inlineStr"/>
+      <c r="R244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -10557,6 +10941,7 @@
         </is>
       </c>
       <c r="Q245" t="inlineStr"/>
+      <c r="R245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -10589,10 +10974,10 @@
       <c r="L246" t="inlineStr"/>
       <c r="M246" t="inlineStr"/>
       <c r="N246" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O246" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P246" t="inlineStr">
         <is>
@@ -10600,6 +10985,7 @@
         </is>
       </c>
       <c r="Q246" t="inlineStr"/>
+      <c r="R246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -10643,6 +11029,7 @@
         </is>
       </c>
       <c r="Q247" t="inlineStr"/>
+      <c r="R247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -10688,6 +11075,7 @@
         </is>
       </c>
       <c r="Q248" t="inlineStr"/>
+      <c r="R248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -10733,6 +11121,7 @@
         </is>
       </c>
       <c r="Q249" t="inlineStr"/>
+      <c r="R249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -10778,6 +11167,7 @@
         </is>
       </c>
       <c r="Q250" t="inlineStr"/>
+      <c r="R250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -10823,6 +11213,7 @@
         </is>
       </c>
       <c r="Q251" t="inlineStr"/>
+      <c r="R251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -10858,6 +11249,7 @@
         </is>
       </c>
       <c r="Q252" t="inlineStr"/>
+      <c r="R252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -10893,6 +11285,7 @@
         </is>
       </c>
       <c r="Q253" t="inlineStr"/>
+      <c r="R253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -10928,6 +11321,7 @@
         </is>
       </c>
       <c r="Q254" t="inlineStr"/>
+      <c r="R254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -10963,6 +11357,7 @@
         </is>
       </c>
       <c r="Q255" t="inlineStr"/>
+      <c r="R255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -11008,6 +11403,7 @@
         </is>
       </c>
       <c r="Q256" t="inlineStr"/>
+      <c r="R256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -11053,6 +11449,7 @@
         </is>
       </c>
       <c r="Q257" t="inlineStr"/>
+      <c r="R257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -11085,10 +11482,10 @@
       <c r="L258" t="inlineStr"/>
       <c r="M258" t="inlineStr"/>
       <c r="N258" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O258" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P258" t="inlineStr">
         <is>
@@ -11096,6 +11493,7 @@
         </is>
       </c>
       <c r="Q258" t="inlineStr"/>
+      <c r="R258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -11139,6 +11537,7 @@
         </is>
       </c>
       <c r="Q259" t="inlineStr"/>
+      <c r="R259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -11184,6 +11583,7 @@
         </is>
       </c>
       <c r="Q260" t="inlineStr"/>
+      <c r="R260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -11229,6 +11629,7 @@
         </is>
       </c>
       <c r="Q261" t="inlineStr"/>
+      <c r="R261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -11274,6 +11675,7 @@
         </is>
       </c>
       <c r="Q262" t="inlineStr"/>
+      <c r="R262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -11319,6 +11721,7 @@
         </is>
       </c>
       <c r="Q263" t="inlineStr"/>
+      <c r="R263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -11354,6 +11757,7 @@
         </is>
       </c>
       <c r="Q264" t="inlineStr"/>
+      <c r="R264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -11389,6 +11793,7 @@
         </is>
       </c>
       <c r="Q265" t="inlineStr"/>
+      <c r="R265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -11424,6 +11829,7 @@
         </is>
       </c>
       <c r="Q266" t="inlineStr"/>
+      <c r="R266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -11459,6 +11865,7 @@
         </is>
       </c>
       <c r="Q267" t="inlineStr"/>
+      <c r="R267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -11504,6 +11911,7 @@
         </is>
       </c>
       <c r="Q268" t="inlineStr"/>
+      <c r="R268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -11549,6 +11957,7 @@
         </is>
       </c>
       <c r="Q269" t="inlineStr"/>
+      <c r="R269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -11581,10 +11990,10 @@
       <c r="L270" t="inlineStr"/>
       <c r="M270" t="inlineStr"/>
       <c r="N270" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O270" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P270" t="inlineStr">
         <is>
@@ -11592,6 +12001,7 @@
         </is>
       </c>
       <c r="Q270" t="inlineStr"/>
+      <c r="R270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -11635,6 +12045,7 @@
         </is>
       </c>
       <c r="Q271" t="inlineStr"/>
+      <c r="R271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -11680,6 +12091,7 @@
         </is>
       </c>
       <c r="Q272" t="inlineStr"/>
+      <c r="R272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -11725,6 +12137,7 @@
         </is>
       </c>
       <c r="Q273" t="inlineStr"/>
+      <c r="R273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -11770,6 +12183,7 @@
         </is>
       </c>
       <c r="Q274" t="inlineStr"/>
+      <c r="R274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -11815,6 +12229,7 @@
         </is>
       </c>
       <c r="Q275" t="inlineStr"/>
+      <c r="R275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -11850,6 +12265,7 @@
         </is>
       </c>
       <c r="Q276" t="inlineStr"/>
+      <c r="R276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -11885,6 +12301,7 @@
         </is>
       </c>
       <c r="Q277" t="inlineStr"/>
+      <c r="R277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -11920,6 +12337,7 @@
         </is>
       </c>
       <c r="Q278" t="inlineStr"/>
+      <c r="R278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -11955,6 +12373,7 @@
         </is>
       </c>
       <c r="Q279" t="inlineStr"/>
+      <c r="R279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -12000,6 +12419,7 @@
         </is>
       </c>
       <c r="Q280" t="inlineStr"/>
+      <c r="R280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -12045,6 +12465,7 @@
         </is>
       </c>
       <c r="Q281" t="inlineStr"/>
+      <c r="R281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -12077,10 +12498,10 @@
       <c r="L282" t="inlineStr"/>
       <c r="M282" t="inlineStr"/>
       <c r="N282" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O282" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P282" t="inlineStr">
         <is>
@@ -12088,6 +12509,7 @@
         </is>
       </c>
       <c r="Q282" t="inlineStr"/>
+      <c r="R282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -12131,6 +12553,7 @@
         </is>
       </c>
       <c r="Q283" t="inlineStr"/>
+      <c r="R283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -12176,6 +12599,7 @@
         </is>
       </c>
       <c r="Q284" t="inlineStr"/>
+      <c r="R284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -12221,6 +12645,7 @@
         </is>
       </c>
       <c r="Q285" t="inlineStr"/>
+      <c r="R285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -12266,6 +12691,7 @@
         </is>
       </c>
       <c r="Q286" t="inlineStr"/>
+      <c r="R286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -12311,6 +12737,7 @@
         </is>
       </c>
       <c r="Q287" t="inlineStr"/>
+      <c r="R287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -12346,6 +12773,7 @@
         </is>
       </c>
       <c r="Q288" t="inlineStr"/>
+      <c r="R288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -12381,6 +12809,7 @@
         </is>
       </c>
       <c r="Q289" t="inlineStr"/>
+      <c r="R289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -12416,6 +12845,7 @@
         </is>
       </c>
       <c r="Q290" t="inlineStr"/>
+      <c r="R290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -12451,6 +12881,7 @@
         </is>
       </c>
       <c r="Q291" t="inlineStr"/>
+      <c r="R291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -12496,6 +12927,7 @@
         </is>
       </c>
       <c r="Q292" t="inlineStr"/>
+      <c r="R292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -12541,6 +12973,7 @@
         </is>
       </c>
       <c r="Q293" t="inlineStr"/>
+      <c r="R293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -12573,10 +13006,10 @@
       <c r="L294" t="inlineStr"/>
       <c r="M294" t="inlineStr"/>
       <c r="N294" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O294" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P294" t="inlineStr">
         <is>
@@ -12584,6 +13017,7 @@
         </is>
       </c>
       <c r="Q294" t="inlineStr"/>
+      <c r="R294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -12627,6 +13061,7 @@
         </is>
       </c>
       <c r="Q295" t="inlineStr"/>
+      <c r="R295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -12672,6 +13107,7 @@
         </is>
       </c>
       <c r="Q296" t="inlineStr"/>
+      <c r="R296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -12717,6 +13153,7 @@
         </is>
       </c>
       <c r="Q297" t="inlineStr"/>
+      <c r="R297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -12762,6 +13199,7 @@
         </is>
       </c>
       <c r="Q298" t="inlineStr"/>
+      <c r="R298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -12807,6 +13245,7 @@
         </is>
       </c>
       <c r="Q299" t="inlineStr"/>
+      <c r="R299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -12842,6 +13281,7 @@
         </is>
       </c>
       <c r="Q300" t="inlineStr"/>
+      <c r="R300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -12877,6 +13317,7 @@
         </is>
       </c>
       <c r="Q301" t="inlineStr"/>
+      <c r="R301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -12912,6 +13353,7 @@
         </is>
       </c>
       <c r="Q302" t="inlineStr"/>
+      <c r="R302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -12947,6 +13389,7 @@
         </is>
       </c>
       <c r="Q303" t="inlineStr"/>
+      <c r="R303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -12992,6 +13435,7 @@
         </is>
       </c>
       <c r="Q304" t="inlineStr"/>
+      <c r="R304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -13037,6 +13481,7 @@
         </is>
       </c>
       <c r="Q305" t="inlineStr"/>
+      <c r="R305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -13069,10 +13514,10 @@
       <c r="L306" t="inlineStr"/>
       <c r="M306" t="inlineStr"/>
       <c r="N306" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O306" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P306" t="inlineStr">
         <is>
@@ -13080,6 +13525,7 @@
         </is>
       </c>
       <c r="Q306" t="inlineStr"/>
+      <c r="R306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -13123,6 +13569,7 @@
         </is>
       </c>
       <c r="Q307" t="inlineStr"/>
+      <c r="R307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -13168,6 +13615,7 @@
         </is>
       </c>
       <c r="Q308" t="inlineStr"/>
+      <c r="R308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -13213,6 +13661,7 @@
         </is>
       </c>
       <c r="Q309" t="inlineStr"/>
+      <c r="R309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -13258,6 +13707,7 @@
         </is>
       </c>
       <c r="Q310" t="inlineStr"/>
+      <c r="R310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -13303,6 +13753,7 @@
         </is>
       </c>
       <c r="Q311" t="inlineStr"/>
+      <c r="R311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -13338,6 +13789,7 @@
         </is>
       </c>
       <c r="Q312" t="inlineStr"/>
+      <c r="R312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -13373,6 +13825,7 @@
         </is>
       </c>
       <c r="Q313" t="inlineStr"/>
+      <c r="R313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -13408,6 +13861,7 @@
         </is>
       </c>
       <c r="Q314" t="inlineStr"/>
+      <c r="R314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -13443,6 +13897,7 @@
         </is>
       </c>
       <c r="Q315" t="inlineStr"/>
+      <c r="R315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -13488,6 +13943,7 @@
         </is>
       </c>
       <c r="Q316" t="inlineStr"/>
+      <c r="R316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -13533,6 +13989,7 @@
         </is>
       </c>
       <c r="Q317" t="inlineStr"/>
+      <c r="R317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -13565,10 +14022,10 @@
       <c r="L318" t="inlineStr"/>
       <c r="M318" t="inlineStr"/>
       <c r="N318" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O318" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P318" t="inlineStr">
         <is>
@@ -13576,6 +14033,7 @@
         </is>
       </c>
       <c r="Q318" t="inlineStr"/>
+      <c r="R318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -13619,6 +14077,7 @@
         </is>
       </c>
       <c r="Q319" t="inlineStr"/>
+      <c r="R319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -13664,6 +14123,7 @@
         </is>
       </c>
       <c r="Q320" t="inlineStr"/>
+      <c r="R320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -13709,6 +14169,7 @@
         </is>
       </c>
       <c r="Q321" t="inlineStr"/>
+      <c r="R321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -13754,6 +14215,7 @@
         </is>
       </c>
       <c r="Q322" t="inlineStr"/>
+      <c r="R322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -13799,6 +14261,7 @@
         </is>
       </c>
       <c r="Q323" t="inlineStr"/>
+      <c r="R323" t="inlineStr"/>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -13834,6 +14297,7 @@
         </is>
       </c>
       <c r="Q324" t="inlineStr"/>
+      <c r="R324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -13869,6 +14333,7 @@
         </is>
       </c>
       <c r="Q325" t="inlineStr"/>
+      <c r="R325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -13904,6 +14369,7 @@
         </is>
       </c>
       <c r="Q326" t="inlineStr"/>
+      <c r="R326" t="inlineStr"/>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -13939,6 +14405,7 @@
         </is>
       </c>
       <c r="Q327" t="inlineStr"/>
+      <c r="R327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -13984,6 +14451,7 @@
         </is>
       </c>
       <c r="Q328" t="inlineStr"/>
+      <c r="R328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -14023,6 +14491,7 @@
         </is>
       </c>
       <c r="Q329" t="inlineStr"/>
+      <c r="R329" t="inlineStr"/>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -14055,10 +14524,10 @@
       <c r="L330" t="inlineStr"/>
       <c r="M330" t="inlineStr"/>
       <c r="N330" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O330" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P330" t="inlineStr">
         <is>
@@ -14066,6 +14535,7 @@
         </is>
       </c>
       <c r="Q330" t="inlineStr"/>
+      <c r="R330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -14109,6 +14579,7 @@
         </is>
       </c>
       <c r="Q331" t="inlineStr"/>
+      <c r="R331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -14154,6 +14625,7 @@
         </is>
       </c>
       <c r="Q332" t="inlineStr"/>
+      <c r="R332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -14199,6 +14671,7 @@
         </is>
       </c>
       <c r="Q333" t="inlineStr"/>
+      <c r="R333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -14238,6 +14711,7 @@
         </is>
       </c>
       <c r="Q334" t="inlineStr"/>
+      <c r="R334" t="inlineStr"/>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -14277,6 +14751,7 @@
         </is>
       </c>
       <c r="Q335" t="inlineStr"/>
+      <c r="R335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -14312,6 +14787,7 @@
         </is>
       </c>
       <c r="Q336" t="inlineStr"/>
+      <c r="R336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -14347,6 +14823,7 @@
         </is>
       </c>
       <c r="Q337" t="inlineStr"/>
+      <c r="R337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -14382,6 +14859,7 @@
         </is>
       </c>
       <c r="Q338" t="inlineStr"/>
+      <c r="R338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -14417,6 +14895,7 @@
         </is>
       </c>
       <c r="Q339" t="inlineStr"/>
+      <c r="R339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -14462,6 +14941,7 @@
         </is>
       </c>
       <c r="Q340" t="inlineStr"/>
+      <c r="R340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -14501,6 +14981,7 @@
         </is>
       </c>
       <c r="Q341" t="inlineStr"/>
+      <c r="R341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -14533,10 +15014,10 @@
       <c r="L342" t="inlineStr"/>
       <c r="M342" t="inlineStr"/>
       <c r="N342" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O342" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P342" t="inlineStr">
         <is>
@@ -14544,6 +15025,7 @@
         </is>
       </c>
       <c r="Q342" t="inlineStr"/>
+      <c r="R342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -14587,6 +15069,7 @@
         </is>
       </c>
       <c r="Q343" t="inlineStr"/>
+      <c r="R343" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -14632,6 +15115,7 @@
         </is>
       </c>
       <c r="Q344" t="inlineStr"/>
+      <c r="R344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -14677,6 +15161,7 @@
         </is>
       </c>
       <c r="Q345" t="inlineStr"/>
+      <c r="R345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -14716,6 +15201,7 @@
         </is>
       </c>
       <c r="Q346" t="inlineStr"/>
+      <c r="R346" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -14755,6 +15241,7 @@
         </is>
       </c>
       <c r="Q347" t="inlineStr"/>
+      <c r="R347" t="inlineStr"/>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -14790,6 +15277,7 @@
         </is>
       </c>
       <c r="Q348" t="inlineStr"/>
+      <c r="R348" t="inlineStr"/>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -14825,6 +15313,7 @@
         </is>
       </c>
       <c r="Q349" t="inlineStr"/>
+      <c r="R349" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -14860,6 +15349,7 @@
         </is>
       </c>
       <c r="Q350" t="inlineStr"/>
+      <c r="R350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -14895,6 +15385,7 @@
         </is>
       </c>
       <c r="Q351" t="inlineStr"/>
+      <c r="R351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -14934,6 +15425,7 @@
         </is>
       </c>
       <c r="Q352" t="inlineStr"/>
+      <c r="R352" t="inlineStr"/>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -14979,6 +15471,7 @@
         </is>
       </c>
       <c r="Q353" t="inlineStr"/>
+      <c r="R353" t="inlineStr"/>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -15011,10 +15504,10 @@
       <c r="L354" t="inlineStr"/>
       <c r="M354" t="inlineStr"/>
       <c r="N354" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O354" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P354" t="inlineStr">
         <is>
@@ -15022,6 +15515,7 @@
         </is>
       </c>
       <c r="Q354" t="inlineStr"/>
+      <c r="R354" t="inlineStr"/>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -15065,6 +15559,7 @@
         </is>
       </c>
       <c r="Q355" t="inlineStr"/>
+      <c r="R355" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -15104,6 +15599,7 @@
         </is>
       </c>
       <c r="Q356" t="inlineStr"/>
+      <c r="R356" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -15143,6 +15639,7 @@
         </is>
       </c>
       <c r="Q357" t="inlineStr"/>
+      <c r="R357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -15188,6 +15685,7 @@
         </is>
       </c>
       <c r="Q358" t="inlineStr"/>
+      <c r="R358" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -15233,6 +15731,7 @@
         </is>
       </c>
       <c r="Q359" t="inlineStr"/>
+      <c r="R359" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -15268,6 +15767,7 @@
         </is>
       </c>
       <c r="Q360" t="inlineStr"/>
+      <c r="R360" t="inlineStr"/>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -15303,6 +15803,7 @@
         </is>
       </c>
       <c r="Q361" t="inlineStr"/>
+      <c r="R361" t="inlineStr"/>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -15338,6 +15839,7 @@
         </is>
       </c>
       <c r="Q362" t="inlineStr"/>
+      <c r="R362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -15373,6 +15875,7 @@
         </is>
       </c>
       <c r="Q363" t="inlineStr"/>
+      <c r="R363" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -15412,6 +15915,7 @@
         </is>
       </c>
       <c r="Q364" t="inlineStr"/>
+      <c r="R364" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -15457,6 +15961,7 @@
         </is>
       </c>
       <c r="Q365" t="inlineStr"/>
+      <c r="R365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -15489,10 +15994,10 @@
       <c r="L366" t="inlineStr"/>
       <c r="M366" t="inlineStr"/>
       <c r="N366" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O366" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P366" t="inlineStr">
         <is>
@@ -15500,6 +16005,7 @@
         </is>
       </c>
       <c r="Q366" t="inlineStr"/>
+      <c r="R366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -15543,6 +16049,7 @@
         </is>
       </c>
       <c r="Q367" t="inlineStr"/>
+      <c r="R367" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -15582,6 +16089,7 @@
         </is>
       </c>
       <c r="Q368" t="inlineStr"/>
+      <c r="R368" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -15621,6 +16129,7 @@
         </is>
       </c>
       <c r="Q369" t="inlineStr"/>
+      <c r="R369" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -15666,6 +16175,7 @@
         </is>
       </c>
       <c r="Q370" t="inlineStr"/>
+      <c r="R370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -15711,6 +16221,7 @@
         </is>
       </c>
       <c r="Q371" t="inlineStr"/>
+      <c r="R371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -15746,6 +16257,7 @@
         </is>
       </c>
       <c r="Q372" t="inlineStr"/>
+      <c r="R372" t="inlineStr"/>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -15781,6 +16293,7 @@
         </is>
       </c>
       <c r="Q373" t="inlineStr"/>
+      <c r="R373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -15816,6 +16329,7 @@
         </is>
       </c>
       <c r="Q374" t="inlineStr"/>
+      <c r="R374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -15851,6 +16365,7 @@
         </is>
       </c>
       <c r="Q375" t="inlineStr"/>
+      <c r="R375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -15890,6 +16405,7 @@
         </is>
       </c>
       <c r="Q376" t="inlineStr"/>
+      <c r="R376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -15935,6 +16451,7 @@
         </is>
       </c>
       <c r="Q377" t="inlineStr"/>
+      <c r="R377" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -15967,10 +16484,10 @@
       <c r="L378" t="inlineStr"/>
       <c r="M378" t="inlineStr"/>
       <c r="N378" t="n">
-        <v>4.981448916616301</v>
+        <v>5.003037840566488</v>
       </c>
       <c r="O378" t="n">
-        <v>0.2416045425067761</v>
+        <v>0.123267623727947</v>
       </c>
       <c r="P378" t="inlineStr">
         <is>
@@ -15978,6 +16495,7 @@
         </is>
       </c>
       <c r="Q378" t="inlineStr"/>
+      <c r="R378" t="inlineStr"/>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -16021,6 +16539,7 @@
         </is>
       </c>
       <c r="Q379" t="inlineStr"/>
+      <c r="R379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -16060,6 +16579,7 @@
         </is>
       </c>
       <c r="Q380" t="inlineStr"/>
+      <c r="R380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -16099,6 +16619,7 @@
         </is>
       </c>
       <c r="Q381" t="inlineStr"/>
+      <c r="R381" t="inlineStr"/>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -16144,6 +16665,7 @@
         </is>
       </c>
       <c r="Q382" t="inlineStr"/>
+      <c r="R382" t="inlineStr"/>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -16189,6 +16711,7 @@
         </is>
       </c>
       <c r="Q383" t="inlineStr"/>
+      <c r="R383" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -16224,6 +16747,7 @@
         </is>
       </c>
       <c r="Q384" t="inlineStr"/>
+      <c r="R384" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>